<commit_message>
feat: get taxiing time for each gate
</commit_message>
<xml_diff>
--- a/data/mintaxitime.xlsx
+++ b/data/mintaxitime.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pycharm\GAP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3035CE6-60D8-46A5-B417-282B56AF0E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C775872-8737-4591-8D28-B043E969A84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2436" yWindow="1380" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="mintaxitime " sheetId="1" r:id="rId2"/>
+    <sheet name="mintaxitime" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">sheet1!$A$1:$M$167</definedName>
@@ -2197,7 +2197,21 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表_表1" displayName="表_表1" ref="A1:M167" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:M167" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <autoFilter ref="A1:M167" xr:uid="{00000000-0009-0000-0100-000002000000}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
+    <filterColumn colId="11" hiddenButton="1"/>
+    <filterColumn colId="12" hiddenButton="1"/>
+  </autoFilter>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name=" ZBTJ      ZBTJ_PN     .1" queryTableFieldId="1" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name=" ZBTJ      ZBTJ_PN     .2" queryTableFieldId="2" dataDxfId="11"/>
@@ -2213,7 +2227,7 @@
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" uniqueName="12" name=" ZBTJ      ZBTJ_PN     .12" queryTableFieldId="12" dataDxfId="1"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" uniqueName="13" name=" ZBTJ      ZBTJ_PN     .13" queryTableFieldId="13" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2528,8 +2542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M167"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -9399,7 +9413,7 @@
   <dimension ref="A1:A167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>